<commit_message>
Update data files - Bot run at 2026-02-12 17:10:17 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1821,9 +1821,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2026-02-12T17:10:09.710764+00:00</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>['16:48-17:50']</t>
@@ -1833,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1848,7 +1852,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[224, 204, 169, 304]</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 07:36:48 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1556,7 +1556,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2026-02-13T07:32:55.202461+00:00</t>
+          <t>2026-02-13T07:36:43.231386+00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>[19, 32, 25, 15]</t>
+          <t>[19, 32, 25, 15, 132, 127]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 17:25:04 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1279,11 +1279,11 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2026-02-12T10:38:35.663179+00:00</t>
+          <t>2026-02-13T17:24:59.479592+00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" t="n">
         <v>2</v>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[169, 425, 439, 442, 438]</t>
+          <t>[169, 425, 439, 442, 438, 272222]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 22:00:39 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,67 +434,67 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>group_name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>join_date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>current_phase</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>last_action_date</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>time_ranges</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>link_enabled</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>reactions_count</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>replies_count</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>posts_count</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>reacted_message_ids</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>replied_message_ids</t>
         </is>
@@ -617,7 +629,11 @@
       <c r="D4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2026-02-13T22:00:33.459316+00:00</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>['22:00-22:40']</t>
@@ -627,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -642,7 +658,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[31176, 31174]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 22:47:39 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -686,7 +686,11 @@
       <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2026-02-13T22:47:35.512581+00:00</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>['22:40-23:20']</t>
@@ -696,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -711,7 +715,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[155336]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 07:37:45 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1220,7 +1220,11 @@
       <c r="D15" t="n">
         <v>1</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2026-02-14T07:37:41.028776+00:00</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>['07:20-08:00']</t>
@@ -1230,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1245,7 +1249,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[136, 155]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 08:39:02 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1277,7 +1277,11 @@
       <c r="D16" t="n">
         <v>1</v>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2026-02-14T08:38:49.540574+00:00</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>['08:00-08:40']</t>
@@ -1287,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1302,7 +1306,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[101305]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 09:36:48 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1387,7 +1387,11 @@
       <c r="D18" t="n">
         <v>1</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2026-02-14T09:36:43.258436+00:00</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>['09:20-10:00']</t>
@@ -1397,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1412,7 +1416,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[14686, 14706]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 12:59:28 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -955,7 +955,11 @@
       <c r="D10" t="n">
         <v>1</v>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2026-02-14T12:59:23.676451+00:00</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>['12:30-13:20']</t>
@@ -965,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -980,7 +984,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[24554, 24546, 24552]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 17:29:53 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -519,7 +519,11 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2026-02-14T17:29:45.947226+00:00</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>['17:00-19:30']</t>
@@ -529,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -544,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[272285, 272284, 272296, 272297]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 17:53:25 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-14T17:29:45.947226+00:00</t>
+          <t>2026-02-14T17:53:16.847547+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297]</t>
+          <t>[272285, 272284, 272296, 272297, 272295]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 18:41:55 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-14T17:53:16.847547+00:00</t>
+          <t>2026-02-14T18:41:49.318335+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 19:28:35 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-14T18:41:49.318335+00:00</t>
+          <t>2026-02-14T19:28:28.976393+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 19:48:22 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-13T19:57:08.907330+00:00</t>
+          <t>2026-02-14T19:48:17.392963+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002]</t>
+          <t>[486988, 486982, 487002, 487051]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 20:32:48 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-14T19:48:17.392963+00:00</t>
+          <t>2026-02-14T20:32:43.125732+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 22:29:31 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -635,7 +635,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-13T22:00:33.459316+00:00</t>
+          <t>2026-02-14T22:29:25.782939+00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[31176, 31174]</t>
+          <t>[31176, 31174, 31172, 31180]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 22:54:44 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -692,7 +692,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-02-13T22:47:35.512581+00:00</t>
+          <t>2026-02-14T22:54:39.673333+00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[155336]</t>
+          <t>[155336, 155318, 155334, 155338]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 02:42:16 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1664,7 +1664,11 @@
       <c r="D23" t="n">
         <v>1</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2026-02-15T02:42:11.485179+00:00</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>['02:40-03:20']</t>
@@ -1674,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1689,7 +1693,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[18697]</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 04:58:36 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1827,7 +1827,11 @@
       <c r="D26" t="n">
         <v>1</v>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2026-02-15T04:58:30.261418+00:00</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>['04:40-05:20']</t>
@@ -1837,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1852,7 +1856,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[10246]</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 07:22:38 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2026-02-14T07:37:41.028776+00:00</t>
+          <t>2026-02-15T07:22:33.152903+00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[136, 155]</t>
+          <t>[136, 155, 150, 158]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 08:45:51 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1342,7 +1342,11 @@
       <c r="D17" t="n">
         <v>1</v>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2026-02-15T08:45:46.371064+00:00</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>['08:40-09:20']</t>
@@ -1352,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1367,7 +1371,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[191121, 191156]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 11:27:49 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -853,7 +853,11 @@
       <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2026-02-15T11:27:44.666162+00:00</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>['10:50-11:40']</t>
@@ -863,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -878,7 +882,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[67735, 67733]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 13:01:18 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -965,7 +965,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2026-02-14T12:59:23.676451+00:00</t>
+          <t>2026-02-15T13:01:13.846078+00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -992,7 +992,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[24554, 24546, 24552]</t>
+          <t>[24554, 24546, 24552, 24550, 24556]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 14:00:58 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1020,7 +1020,11 @@
       <c r="D11" t="n">
         <v>1</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2026-02-15T14:00:53.237710+00:00</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>['13:20-14:10']</t>
@@ -1030,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1045,7 +1049,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[68050]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 17:30:06 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-14T19:28:28.976393+00:00</t>
+          <t>2026-02-15T17:30:02.176829+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 17:54:52 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-15T17:30:02.176829+00:00</t>
+          <t>2026-02-15T17:54:45.236771+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 18:42:54 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-15T17:54:45.236771+00:00</t>
+          <t>2026-02-15T18:42:46.162432+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 19:30:56 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-14T20:32:43.125732+00:00</t>
+          <t>2026-02-15T19:30:51.144983+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 21:30:15 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-15T19:30:51.144983+00:00</t>
+          <t>2026-02-15T21:30:09.702382+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 22:30:33 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -635,7 +635,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-14T22:29:25.782939+00:00</t>
+          <t>2026-02-15T22:30:27.546357+00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[31176, 31174, 31172, 31180]</t>
+          <t>[31176, 31174, 31172, 31180, 31181, 31175]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-15 23:34:10 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -747,7 +747,11 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2026-02-15T23:34:04.656313+00:00</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>['23:20-24:00']</t>
@@ -757,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -772,7 +776,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[138847, 138848]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 06:41:39 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1187,7 +1187,11 @@
       <c r="D14" t="n">
         <v>1</v>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2026-02-16T06:41:33.041823+00:00</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>['06:40-07:20']</t>
@@ -1197,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1212,7 +1216,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[14475, 14480]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 09:01:09 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1360,7 +1360,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2026-02-15T08:45:46.371064+00:00</t>
+          <t>2026-02-16T09:01:03.946740+00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[191121, 191156]</t>
+          <t>[191121, 191156, 191185, 191125]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 11:24:21 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -859,7 +859,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2026-02-15T11:27:44.666162+00:00</t>
+          <t>2026-02-16T11:24:16.148630+00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -886,7 +886,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[67735, 67733]</t>
+          <t>[67735, 67733, 67737, 67734]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 13:47:19 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2026-02-15T14:00:53.237710+00:00</t>
+          <t>2026-02-16T13:47:13.779669+00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[68050]</t>
+          <t>[68050, 68073, 68060, 68065]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 17:41:42 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-15T18:42:46.162432+00:00</t>
+          <t>2026-02-16T17:41:36.922091+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 18:52:11 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-16T17:41:36.922091+00:00</t>
+          <t>2026-02-16T18:52:05.939922+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 19:35:11 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-15T21:30:09.702382+00:00</t>
+          <t>2026-02-16T19:35:06.620522+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 20:37:36 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-16T19:35:06.620522+00:00</t>
+          <t>2026-02-16T20:37:31.972406+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 21:34:17 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-16T20:37:31.972406+00:00</t>
+          <t>2026-02-16T21:34:10.896615+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 22:35:03 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -635,7 +635,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-15T22:30:27.546357+00:00</t>
+          <t>2026-02-16T22:34:58.045796+00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[31176, 31174, 31172, 31180, 31181, 31175]</t>
+          <t>[31176, 31174, 31172, 31180, 31181, 31175, 31177, 31188]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-16 23:34:55 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -749,7 +749,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-02-15T23:34:04.656313+00:00</t>
+          <t>2026-02-16T23:34:50.937210+00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -776,7 +776,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[138847, 138848]</t>
+          <t>[138847, 138848, 138887, 138886, 138850, 138866]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 08:54:24 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1360,7 +1360,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2026-02-16T09:01:03.946740+00:00</t>
+          <t>2026-02-17T08:54:19.542385+00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[191121, 191156, 191185, 191125]</t>
+          <t>[191121, 191156, 191185, 191125, 191187]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 13:14:24 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -969,7 +969,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2026-02-15T13:01:13.846078+00:00</t>
+          <t>2026-02-17T13:14:18.640584+00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[24554, 24546, 24552, 24550, 24556]</t>
+          <t>[24554, 24546, 24552, 24550, 24556, 24577]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 17:57:13 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-16T18:52:05.939922+00:00</t>
+          <t>2026-02-17T17:57:08.258390+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 19:09:18 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-17T17:57:08.258390+00:00</t>
+          <t>2026-02-17T19:09:12.343668+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 21:04:34 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-16T21:34:10.896615+00:00</t>
+          <t>2026-02-17T21:04:28.868833+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159, 487228, 487218, 487227]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 22:41:00 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -692,7 +692,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-02-14T22:54:39.673333+00:00</t>
+          <t>2026-02-17T22:40:54.602744+00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[155336, 155318, 155334, 155338]</t>
+          <t>[155336, 155318, 155334, 155338, 155410, 155432]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-17 23:34:45 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -749,7 +749,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-02-16T23:34:50.937210+00:00</t>
+          <t>2026-02-17T23:34:41.137869+00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -776,7 +776,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[138847, 138848, 138887, 138886, 138850, 138866]</t>
+          <t>[138847, 138848, 138887, 138886, 138850, 138866, 138914]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 02:37:24 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1631,7 +1631,11 @@
       <c r="D22" t="n">
         <v>1</v>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2026-02-18T02:37:18.786360+00:00</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>['02:00-02:40']</t>
@@ -1641,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1656,7 +1660,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[32523]</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 07:34:08 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1246,7 +1246,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2026-02-15T07:22:33.152903+00:00</t>
+          <t>2026-02-18T07:34:04.340098+00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[136, 155, 150, 158]</t>
+          <t>[136, 155, 150, 158, 142, 140]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 08:53:17 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1360,7 +1360,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2026-02-17T08:54:19.542385+00:00</t>
+          <t>2026-02-18T08:53:11.470929+00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[191121, 191156, 191185, 191125, 191187]</t>
+          <t>[191121, 191156, 191185, 191125, 191187, 191205]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 10:52:47 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -859,7 +859,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2026-02-16T11:24:16.148630+00:00</t>
+          <t>2026-02-18T10:52:43.183122+00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -886,7 +886,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[67735, 67733, 67737, 67734]</t>
+          <t>[67735, 67733, 67737, 67734, 67742, 67743]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 13:16:00 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -969,7 +969,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2026-02-17T13:14:18.640584+00:00</t>
+          <t>2026-02-18T13:15:54.658103+00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[24554, 24546, 24552, 24550, 24556, 24577]</t>
+          <t>[24554, 24546, 24552, 24550, 24556, 24577, 24590, 24581]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 17:53:58 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-17T19:09:12.343668+00:00</t>
+          <t>2026-02-18T17:53:51.259222+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 19:02:18 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-18T17:53:51.259222+00:00</t>
+          <t>2026-02-18T19:02:13.650830+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 20:04:03 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -574,11 +574,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-17T21:04:28.868833+00:00</t>
+          <t>2026-02-18T20:03:57.516403+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159, 487228, 487218, 487227]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159, 487228, 487218, 487227, 487257]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 08:53:01 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1356,11 +1356,11 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:11.470929+00:00</t>
+          <t>2026-02-19T08:52:56.717571+00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[191121, 191156, 191185, 191125, 191187, 191205]</t>
+          <t>[191121, 191156, 191185, 191125, 191187, 191205, 191213]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 23:35:12 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -749,7 +749,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-02-17T23:34:41.137869+00:00</t>
+          <t>2026-02-19T23:35:06.585741+00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -776,7 +776,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[138847, 138848, 138887, 138886, 138850, 138866, 138914]</t>
+          <t>[138847, 138848, 138887, 138886, 138850, 138866, 138914, 138933]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 18:04:29 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-20T17:08:34.810828+00:00</t>
+          <t>2026-02-20T18:04:24.242267+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 22:32:36 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -635,7 +635,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-16T22:34:58.045796+00:00</t>
+          <t>2026-02-20T22:32:31.951603+00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[31176, 31174, 31172, 31180, 31181, 31175, 31177, 31188]</t>
+          <t>[31176, 31174, 31172, 31180, 31181, 31175, 31177, 31188, 31201, 31202]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 17:54:19 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-21T17:29:47.682284+00:00</t>
+          <t>2026-02-21T17:54:14.065332+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771, 272773, 272770, 272775]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 18:42:12 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-21T17:54:14.065332+00:00</t>
+          <t>2026-02-21T18:42:05.734255+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771, 272773, 272770, 272775]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771, 272773, 272770, 272775, 272772]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 19:29:15 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-21T18:42:05.734255+00:00</t>
+          <t>2026-02-21T19:29:09.821390+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771, 272773, 272770, 272775, 272772]</t>
+          <t>[272285, 272284, 272296, 272297, 272295, 272303, 272301, 272305, 272302, 272312, 272313, 272308, 272315, 272316, 272304, 272399, 272407, 272403, 272405, 272408, 272413, 272490, 272501, 272500, 272592, 272600, 272605, 272601, 272610, 272673, 272667, 272674, 272675, 272723, 272729, 272727, 272728, 272771, 272773, 272770, 272775, 272772, 272777, 272779, 272774]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 20:31:04 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -578,7 +578,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-21T19:48:58.899025+00:00</t>
+          <t>2026-02-21T20:31:00.085146+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159, 487228, 487218, 487227, 487257, 487230, 487240, 487291, 487304, 487314, 487315, 487370, 487384, 487372, 487416]</t>
+          <t>[486988, 486982, 487002, 487051, 487036, 487065, 487059, 487110, 487103, 487102, 487114, 487074, 487066, 487055, 487138, 487137, 487149, 487164, 487144, 487159, 487228, 487218, 487227, 487257, 487230, 487240, 487291, 487304, 487314, 487315, 487370, 487384, 487372, 487416, 487434, 487439, 487419, 487433]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 22:54:42 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -692,7 +692,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-02-17T22:40:54.602744+00:00</t>
+          <t>2026-02-21T22:54:38.207266+00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[155336, 155318, 155334, 155338, 155410, 155432]</t>
+          <t>[155336, 155318, 155334, 155338, 155410, 155432, 155554]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 06:55:53 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1193,7 +1193,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2026-02-21T07:08:26.723153+00:00</t>
+          <t>2026-02-22T06:55:47.869157+00:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[14475, 14480, 14522]</t>
+          <t>[14475, 14480, 14522, 14523, 14531]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 07:39:26 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1250,7 +1250,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2026-02-21T07:53:02.577926+00:00</t>
+          <t>2026-02-22T07:39:19.390111+00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[136, 155, 150, 158, 142, 140, 151, 137, 139]</t>
+          <t>[136, 155, 150, 158, 142, 140, 151, 137, 139, 159]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 08:38:42 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1307,7 +1307,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2026-02-20T08:03:27.271167+00:00</t>
+          <t>2026-02-22T08:38:36.786821+00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[101305, 101325, 101324]</t>
+          <t>[101305, 101325, 101324, 101327]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">

</xml_diff>